<commit_message>
fix: grandes arreglos de la interfaz + extraccion de periodos 100% funcional
</commit_message>
<xml_diff>
--- a/Data/Extracto_Validacion2.xlsx
+++ b/Data/Extracto_Validacion2.xlsx
@@ -9,17 +9,11 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Resumen General" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Resumen_Alvear Palace (A)" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tipos_Alvear Palace (A)" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Periodos_Alvear Palace (A)" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Extras_Alvear Palace (A)" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Resumen_Faena Hotel Buenos A" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tipos_Faena Hotel Buenos A" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Periodos_Faena Hotel Buenos A" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Extras_Faena Hotel Buenos A" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Resumen_Four Seasons Buenos " sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tipos_Four Seasons Buenos " sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Periodos_Four Seasons Buenos " sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Extras_Four Seasons Buenos " sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Periodos_Alvear Palace (A)" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Resumen_Faena Hotel Buenos A" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Periodos_Faena Hotel Buenos A" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Resumen_Four Seasons Buenos " sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Periodos_Four Seasons Buenos " sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -46,7 +40,7 @@
       <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -71,18 +65,6 @@
         <bgColor rgb="0070AD47"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00ED7D31"/>
-        <bgColor rgb="00ED7D31"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="009966FF"/>
-        <bgColor rgb="009966FF"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -96,20 +78,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -599,1714 +575,13 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
         <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H41"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="25" customWidth="1" min="1" max="1"/>
-    <col width="30" customWidth="1" min="2" max="2"/>
-    <col width="40" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="60" customWidth="1" min="8" max="8"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="inlineStr">
-        <is>
-          <t>Hotel</t>
-        </is>
-      </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>Tipo</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>Habitación</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>Precio</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>Precio String</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>Row Index</t>
-        </is>
-      </c>
-      <c r="G1" s="3" t="inlineStr">
-        <is>
-          <t>Periodo IDs</t>
-        </is>
-      </c>
-      <c r="H1" s="3" t="inlineStr">
-        <is>
-          <t>Detalles de Periodos</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>dbl/sgl city view guest room w/bb</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>840</v>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="n">
-        <v>194</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-10-2025 - 31-10-2025)</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>dbl/sgl mansion view guest room w/bb</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>880</v>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="n">
-        <v>195</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-10-2025 - 31-10-2025)</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>dbl/sgl e-lounge guest room w/bb</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>906.67</v>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="n">
-        <v>196</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-10-2025 - 31-10-2025)</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>dbl/sgl mansion view junior suite w/bb</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>1020</v>
-      </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="n">
-        <v>197</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-10-2025 - 31-10-2025)</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>dbl/sgl e-lounge junior suite w/bb</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>1060</v>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="n">
-        <v>198</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-10-2025 - 31-10-2025)</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>dbl/sgl city view one bedroom suite w/bb</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>1120</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="n">
-        <v>199</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-10-2025 - 31-10-2025)</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>dbl/sgl mansion view one bedroom suite w/bb</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>1146.67</v>
-      </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="n">
-        <v>200</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-10-2025 - 31-10-2025)</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>dbl/sgl e-lounge one bedroom suite w/bb</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>1320</v>
-      </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="n">
-        <v>201</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-10-2025 - 31-10-2025)</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>dbl/sgl city view guest room w/bb</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>933.33</v>
-      </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="n">
-        <v>204</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-11-2025 - 26-11-2025)</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>dbl/sgl mansion view guest room w/bb</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="n">
-        <v>205</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-11-2025 - 26-11-2025)</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>dbl/sgl e-lounge guest room w/bb</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>1026.67</v>
-      </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="n">
-        <v>206</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-11-2025 - 26-11-2025)</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>dbl/sgl mansion view junior suite w/bb</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>1186.67</v>
-      </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="n">
-        <v>207</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-11-2025 - 26-11-2025)</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>dbl/sgl e-lounge junior suite w/bb</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>1246.67</v>
-      </c>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="n">
-        <v>208</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-11-2025 - 26-11-2025)</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>dbl/sgl city view one bedroom suite w/bb</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>1426.67</v>
-      </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="n">
-        <v>209</v>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-11-2025 - 26-11-2025)</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>dbl/sgl mansion view one bedroom suite w/bb</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>1500</v>
-      </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="n">
-        <v>210</v>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-11-2025 - 26-11-2025)</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>dbl/sgl e-lounge one bedroom suite w/bb</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>1560</v>
-      </c>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="n">
-        <v>211</v>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-11-2025 - 26-11-2025)</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>dbl/sgl city view guest room w/bb</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>806.67</v>
-      </c>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="n">
-        <v>232</v>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (04-01-2026 - 31-03-2026)</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>dbl/sgl mansion view guest room w/bb</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>846.67</v>
-      </c>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="n">
-        <v>233</v>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (04-01-2026 - 31-03-2026)</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>dbl/sgl e-lounge guest room w/bb</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>913.33</v>
-      </c>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="n">
-        <v>234</v>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (04-01-2026 - 31-03-2026)</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>dbl/sgl mansion view junior suite w/bb</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>1060</v>
-      </c>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="n">
-        <v>235</v>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (04-01-2026 - 31-03-2026)</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>dbl/sgl e-lounge junior suite w/bb</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>1106.67</v>
-      </c>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="n">
-        <v>236</v>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (04-01-2026 - 31-03-2026)</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>dbl/sgl city view one bedroom suite w/bb</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>1273.33</v>
-      </c>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="n">
-        <v>237</v>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (04-01-2026 - 31-03-2026)</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>dbl/sgl mansion view one bedroom suite w/bb</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>1326.67</v>
-      </c>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="n">
-        <v>238</v>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (04-01-2026 - 31-03-2026)</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>dbl/sgl e-lounge one bedroom suite w/bb</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>1440</v>
-      </c>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="n">
-        <v>239</v>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (04-01-2026 - 31-03-2026)</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>dbl/sgl city view guest room w/bb</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>726.67</v>
-      </c>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="n">
-        <v>242</v>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-04-2026 - 30-09-2026)</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>dbl/sgl mansion view guest room w/bb</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
-        <v>753.33</v>
-      </c>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="n">
-        <v>243</v>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-04-2026 - 30-09-2026)</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>dbl/sgl e-lounge guest room w/bb</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>793.33</v>
-      </c>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="n">
-        <v>244</v>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-04-2026 - 30-09-2026)</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>dbl/sgl mansion view junior suite w/bb</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>853.33</v>
-      </c>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="n">
-        <v>245</v>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-04-2026 - 30-09-2026)</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>dbl/sgl e-lounge junior suite w/bb</t>
-        </is>
-      </c>
-      <c r="D30" t="n">
-        <v>946.67</v>
-      </c>
-      <c r="E30" t="inlineStr"/>
-      <c r="F30" t="n">
-        <v>246</v>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-04-2026 - 30-09-2026)</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>dbl/sgl city view one bedroom suite w/bb</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
-        <v>993.33</v>
-      </c>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="n">
-        <v>247</v>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-04-2026 - 30-09-2026)</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>dbl/sgl mansion view one bedroom suite w/bb</t>
-        </is>
-      </c>
-      <c r="D32" t="n">
-        <v>1046.67</v>
-      </c>
-      <c r="E32" t="inlineStr"/>
-      <c r="F32" t="n">
-        <v>248</v>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-04-2026 - 30-09-2026)</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>dbl/sgl e-lounge one bedroom suite w/bb</t>
-        </is>
-      </c>
-      <c r="D33" t="n">
-        <v>1073.33</v>
-      </c>
-      <c r="E33" t="inlineStr"/>
-      <c r="F33" t="n">
-        <v>249</v>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-04-2026 - 30-09-2026)</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>dbl/sgl city view guest room w/bb</t>
-        </is>
-      </c>
-      <c r="D34" t="n">
-        <v>886.67</v>
-      </c>
-      <c r="E34" t="inlineStr"/>
-      <c r="F34" t="n">
-        <v>252</v>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-10-2026 - 26-11-2026)</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>dbl/sgl mansion view guest room w/bb</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
-        <v>940</v>
-      </c>
-      <c r="E35" t="inlineStr"/>
-      <c r="F35" t="n">
-        <v>253</v>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-10-2026 - 26-11-2026)</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>dbl/sgl e-lounge guest room w/bb</t>
-        </is>
-      </c>
-      <c r="D36" t="n">
-        <v>966.67</v>
-      </c>
-      <c r="E36" t="inlineStr"/>
-      <c r="F36" t="n">
-        <v>254</v>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-10-2026 - 26-11-2026)</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>dbl/sgl mansion view junior suite w/bb</t>
-        </is>
-      </c>
-      <c r="D37" t="n">
-        <v>1106.67</v>
-      </c>
-      <c r="E37" t="inlineStr"/>
-      <c r="F37" t="n">
-        <v>255</v>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-10-2026 - 26-11-2026)</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>dbl/sgl e-lounge junior suite w/bb</t>
-        </is>
-      </c>
-      <c r="D38" t="n">
-        <v>1153.33</v>
-      </c>
-      <c r="E38" t="inlineStr"/>
-      <c r="F38" t="n">
-        <v>256</v>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-10-2026 - 26-11-2026)</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>dbl/sgl city view one bedroom suite w/bb</t>
-        </is>
-      </c>
-      <c r="D39" t="n">
-        <v>1273.33</v>
-      </c>
-      <c r="E39" t="inlineStr"/>
-      <c r="F39" t="n">
-        <v>257</v>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-10-2026 - 26-11-2026)</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>dbl/sgl mansion view one bedroom suite w/bb</t>
-        </is>
-      </c>
-      <c r="D40" t="n">
-        <v>1326.67</v>
-      </c>
-      <c r="E40" t="inlineStr"/>
-      <c r="F40" t="n">
-        <v>258</v>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-10-2026 - 26-11-2026)</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>(Sin tipo específico)</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>dbl/sgl e-lounge one bedroom suite w/bb</t>
-        </is>
-      </c>
-      <c r="D41" t="n">
-        <v>1453.33</v>
-      </c>
-      <c r="E41" t="inlineStr"/>
-      <c r="F41" t="n">
-        <v>259</v>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (01-10-2026 - 26-11-2026)</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="40" customWidth="1" min="1" max="1"/>
-    <col width="25" customWidth="1" min="2" max="2"/>
-    <col width="80" customWidth="1" min="3" max="3"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="4" t="inlineStr">
-        <is>
-          <t>Tipo de Habitación</t>
-        </is>
-      </c>
-      <c r="B1" s="4" t="inlineStr">
-        <is>
-          <t>Cantidad de Habitaciones</t>
-        </is>
-      </c>
-      <c r="C1" s="4" t="inlineStr">
-        <is>
-          <t>Nombres de Habitaciones</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>(No hay tipos de habitación definidos)</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="inlineStr"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="10" customWidth="1" min="1" max="1"/>
-    <col width="35" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="5" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B1" s="5" t="inlineStr">
-        <is>
-          <t>Nombre</t>
-        </is>
-      </c>
-      <c r="C1" s="5" t="inlineStr">
-        <is>
-          <t>Fecha Inicio</t>
-        </is>
-      </c>
-      <c r="D1" s="5" t="inlineStr">
-        <is>
-          <t>Fecha Fin</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>23</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>SIN NOMBRE DE GRUPO</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>01-10-2025</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>31-10-2025</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>24</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>SIN NOMBRE DE GRUPO</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>01-11-2025</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>26-11-2025</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>25</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>SIN NOMBRE DE GRUPO</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>04-01-2026</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>31-03-2026</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>26</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>SIN NOMBRE DE GRUPO</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>01-04-2026</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>30-09-2026</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>27</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>SIN NOMBRE DE GRUPO</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>01-10-2026</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>26-11-2026</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="25" customWidth="1" min="1" max="1"/>
-    <col width="50" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="6" t="inlineStr">
-        <is>
-          <t>Hotel</t>
-        </is>
-      </c>
-      <c r="B1" s="6" t="inlineStr">
-        <is>
-          <t>Nombre del Extra</t>
-        </is>
-      </c>
-      <c r="C1" s="6" t="inlineStr">
-        <is>
-          <t>Precio</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>ADDITIONAL BED: from 13 years old</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>88.88888888888889</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Four Seasons Buenos Aires (A)</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ADDITIONAL BED: from 13 years old</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>88.88888888888889</v>
       </c>
     </row>
   </sheetData>
@@ -4023,227 +2298,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="40" customWidth="1" min="1" max="1"/>
-    <col width="25" customWidth="1" min="2" max="2"/>
-    <col width="80" customWidth="1" min="3" max="3"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="4" t="inlineStr">
-        <is>
-          <t>Tipo de Habitación</t>
-        </is>
-      </c>
-      <c r="B1" s="4" t="inlineStr">
-        <is>
-          <t>Cantidad de Habitaciones</t>
-        </is>
-      </c>
-      <c r="C1" s="4" t="inlineStr">
-        <is>
-          <t>Nombres de Habitaciones</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>SUITES</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>5</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>sgl/dbl palace premier room (jacuzzi) w/breakfast served at restaurant, sgl/dbl/tpl suite junior (jacuzzi) w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old), tpl suite junior (jacuzzi) w/breakfast served at restaurant (3 ad), sgl/dbl/tpl deluxe suite w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old), tpl deluxe suite w/breakfast served at restaurant (3ad)</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>LOUNGE &amp; LE MIRADOR SUITES</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>sgl/dbl junior suite le mirador w/breakfast served at restaurant, sgl/dbl deluxe suite le mirador w/breakfast served atrestaurant</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>GRAND SUITES</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>sgl/dbl/tpl diplomatic suite w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old), tpl/ cpl diplomatic suite w/breakfast served at restaurant. (2 ad + 2 ch 3-12 years old), sgl/dbl governor suite w/breakfast served at restaurant, sgl/dbl/tpl diplomatic suite prestige w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old), tpl/cpl diplomatic suite prestige w/breakfast served at restaurant. (2 ad + 2 ch 3-12 years old)</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>SUITES</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>5</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>sgl/dbl palace premier room (jacuzzi) w/breakfast served at restaurant, sgl/dbl/tpl suite junior (jacuzzi) w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old), tpl suite junior (jacuzzi) w/breakfast served at restaurant (3 ad), sgl/dbl/tpl deluxe suite w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old), tpl deluxe suite w/breakfast served at restaurant (3ad)</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>LOUNGE &amp; LE MIRADOR SUITES</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>sgl/dbl junior suite le mirador w/breakfast served at restaurant, sgl/dbl deluxe suite le mirador w/breakfast served atrestaurant</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>GRAND SUITES</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>5</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>sgl/dbl/tpl diplomatic suite w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old), tpl/ cpl diplomatic suite w/breakfast served at restaurant. tpl (3 ad) / cdpl (2 ad + 2 ch 3-12 years old) ), sgl/dbl governor suite w/breakfast served at restaurant, sgl/dbl/tpl diplomatic suite prestige w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old), tpl/cpl diplomatic suite prestige w/breakfast served at restaurant. tpl (3 ad) / cdpl (2 ad + 2 ch 3-12 years old) )</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>SUITES</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>5</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>sgl/dbl palace premier room (jacuzzi) w/breakfast served at restaurant, sgl/dbl/tpl suite junior (jacuzzi) w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old), tpl suite junior (jacuzzi) w/breakfast served at restaurant (3 ad), sgl/dbl/tpl deluxe suite w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old), tpl deluxe suite w/breakfast served at restaurant (3ad)</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>LOUNGE &amp; LE MIRADOR SUITES</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>sgl/dbl junior suite le mirador w/breakfast served at restaurant, sgl/dbl deluxe suite le mirador w/breakfast served atrestaurant</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>GRAND SUITES</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>5</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>sgl/dbl/tpl diplomatic suite w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old), tpl/ cpl diplomatic suite w/breakfast served at restaurant. tpl (3 ad) / cdpl (2 ad + 2 ch), sgl/dbl governor suite w/breakfast served at restaurant, sgl/dbl/tpl diplomatic suite prestige w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old), tpl/cpl diplomatic suite prestige w/breakfast served at restaurant. tpl (3 ad) / cdpl (2 ad + 2 ch 3-12 years old) )</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>SUITES</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>5</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>sgl/dbl palace premier room (jacuzzi) w/breakfast served at restaurant, sgl/dbl/tpl suite junior (jacuzzi) w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old), tpl suite junior (jacuzzi) w/breakfast served at restaurant (3 ad), sgl/dbl/tpl deluxe suite w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old), tpl deluxe suite w/breakfast served at restaurant (3ad)</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>LOUNGE &amp; LE MIRADOR SUITES</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>2</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>sgl/dbl junior suite le mirador w/breakfast served at restaurant, sgl/dbl deluxe suite le mirador w/breakfast served atrestaurant</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>GRAND SUITES</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>5</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>sgl/dbl/tpl diplomatic suite w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old), tpl/ cpl diplomatic suite w/breakfast served at restaurant. tpl (3 ad) / cdpl (2 ad + 2 ch), sgl/dbl governor suite w/breakfast served at restaurant, sgl/dbl/tpl diplomatic suite prestige w/breakfast served at restaurant. (2 ad + 1 ch 3-12 years old), tpl/cpl diplomatic suite prestige w/breakfast served at restaurant. tpl (3 ad) / cdpl (2 ad + 2 ch 3-12 years old) )</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4259,22 +2313,22 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Nombre</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Fecha Inicio</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Fecha Fin</t>
         </is>
@@ -4525,63 +2579,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="25" customWidth="1" min="1" max="1"/>
-    <col width="50" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="6" t="inlineStr">
-        <is>
-          <t>Hotel</t>
-        </is>
-      </c>
-      <c r="B1" s="6" t="inlineStr">
-        <is>
-          <t>Nombre del Extra</t>
-        </is>
-      </c>
-      <c r="C1" s="6" t="inlineStr">
-        <is>
-          <t>Precio</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Alvear Palace (A)</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>ADDITIONAL BED: From Suite Junior</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>66.66666666666667</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5522,59 +3520,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="40" customWidth="1" min="1" max="1"/>
-    <col width="25" customWidth="1" min="2" max="2"/>
-    <col width="80" customWidth="1" min="3" max="3"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="4" t="inlineStr">
-        <is>
-          <t>Tipo de Habitación</t>
-        </is>
-      </c>
-      <c r="B1" s="4" t="inlineStr">
-        <is>
-          <t>Cantidad de Habitaciones</t>
-        </is>
-      </c>
-      <c r="C1" s="4" t="inlineStr">
-        <is>
-          <t>Nombres de Habitaciones</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>(No hay tipos de habitación definidos)</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="inlineStr"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5595,22 +3541,22 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Nombre</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Fecha Inicio</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Fecha Fin</t>
         </is>
@@ -5821,13 +3767,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5836,85 +3782,1728 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="25" customWidth="1" min="1" max="1"/>
-    <col width="50" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="40" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="60" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Hotel</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
-        <is>
-          <t>Nombre del Extra</t>
-        </is>
-      </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Tipo</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Habitación</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Precio</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>Precio String</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>Row Index</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>Periodo IDs</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>Detalles de Periodos</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Faena Hotel Buenos Aires (A)</t>
+          <t>Four Seasons Buenos Aires (A)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Adults Nee Year Eve´s Dinner (Per person)</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>525</v>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>dbl/sgl city view guest room w/bb</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>840</v>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="n">
+        <v>194</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025)</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Faena Hotel Buenos Aires (A)</t>
+          <t>Four Seasons Buenos Aires (A)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Childs under 12 years old</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>262.5</v>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>dbl/sgl mansion view guest room w/bb</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>880</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>195</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025)</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Faena Hotel Buenos Aires (A)</t>
+          <t>Four Seasons Buenos Aires (A)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ADDITIONAL BED (For child over 12 years old)</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>111.1111111111111</v>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>dbl/sgl e-lounge guest room w/bb</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>906.67</v>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="n">
+        <v>196</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025)</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Faena Hotel Buenos Aires (A)</t>
+          <t>Four Seasons Buenos Aires (A)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ADDITIONAL BED (For child over 12 years old)</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>111.1111111111111</v>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>dbl/sgl mansion view junior suite w/bb</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1020</v>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="n">
+        <v>197</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>dbl/sgl e-lounge junior suite w/bb</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1060</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="n">
+        <v>198</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>dbl/sgl city view one bedroom suite w/bb</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1120</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="n">
+        <v>199</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>dbl/sgl e-lounge one bedroom suite w/bb</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1320</v>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="n">
+        <v>201</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-10-2025 - 31-10-2025)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>dbl/sgl city view guest room w/bb</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>933.33</v>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="n">
+        <v>204</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>24, 25</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-11-2025 - 26-11-2025) |  (08-12-2025 - 21-12-2025)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>dbl/sgl mansion view guest room w/bb</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="n">
+        <v>205</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>24, 25</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-11-2025 - 26-11-2025) |  (08-12-2025 - 21-12-2025)</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>dbl/sgl e-lounge guest room w/bb</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>1026.67</v>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="n">
+        <v>206</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>24, 25</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-11-2025 - 26-11-2025) |  (08-12-2025 - 21-12-2025)</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>dbl/sgl mansion view junior suite w/bb</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>1186.67</v>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="n">
+        <v>207</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>24, 25</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-11-2025 - 26-11-2025) |  (08-12-2025 - 21-12-2025)</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>dbl/sgl e-lounge junior suite w/bb</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>1246.67</v>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="n">
+        <v>208</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>24, 25</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-11-2025 - 26-11-2025) |  (08-12-2025 - 21-12-2025)</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>dbl/sgl city view one bedroom suite w/bb</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>1426.67</v>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="n">
+        <v>209</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>24, 25</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-11-2025 - 26-11-2025) |  (08-12-2025 - 21-12-2025)</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>dbl/sgl mansion view one bedroom suite w/bb</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1500</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="n">
+        <v>210</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>24, 25</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-11-2025 - 26-11-2025) |  (08-12-2025 - 21-12-2025)</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>dbl/sgl e-lounge one bedroom suite w/bb</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>1560</v>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="n">
+        <v>211</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>24, 25</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-11-2025 - 26-11-2025) |  (08-12-2025 - 21-12-2025)</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>dbl/sgl city view guest room w/bb</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>806.67</v>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="n">
+        <v>232</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (04-01-2026 - 31-03-2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>dbl/sgl mansion view guest room w/bb</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>846.67</v>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="n">
+        <v>233</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (04-01-2026 - 31-03-2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>dbl/sgl e-lounge guest room w/bb</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>913.33</v>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="n">
+        <v>234</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (04-01-2026 - 31-03-2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>dbl/sgl mansion view junior suite w/bb</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>1060</v>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="n">
+        <v>235</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (04-01-2026 - 31-03-2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>dbl/sgl e-lounge junior suite w/bb</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>1106.67</v>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="n">
+        <v>236</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (04-01-2026 - 31-03-2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>dbl/sgl city view one bedroom suite w/bb</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>1273.33</v>
+      </c>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="n">
+        <v>237</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (04-01-2026 - 31-03-2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>dbl/sgl mansion view one bedroom suite w/bb</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>1326.67</v>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="n">
+        <v>238</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (04-01-2026 - 31-03-2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>dbl/sgl e-lounge one bedroom suite w/bb</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>1440</v>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="n">
+        <v>239</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (04-01-2026 - 31-03-2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>dbl/sgl city view guest room w/bb</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>726.67</v>
+      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="n">
+        <v>242</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-04-2026 - 30-09-2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>dbl/sgl mansion view guest room w/bb</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>753.33</v>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="n">
+        <v>243</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-04-2026 - 30-09-2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>dbl/sgl e-lounge guest room w/bb</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>793.33</v>
+      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="n">
+        <v>244</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-04-2026 - 30-09-2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>dbl/sgl mansion view junior suite w/bb</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>853.33</v>
+      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="n">
+        <v>245</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-04-2026 - 30-09-2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>dbl/sgl e-lounge junior suite w/bb</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>946.67</v>
+      </c>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="n">
+        <v>246</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-04-2026 - 30-09-2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>dbl/sgl city view one bedroom suite w/bb</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>993.33</v>
+      </c>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="n">
+        <v>247</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-04-2026 - 30-09-2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>dbl/sgl mansion view one bedroom suite w/bb</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>1046.67</v>
+      </c>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="n">
+        <v>248</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-04-2026 - 30-09-2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>dbl/sgl e-lounge one bedroom suite w/bb</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>1073.33</v>
+      </c>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="n">
+        <v>249</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-04-2026 - 30-09-2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>dbl/sgl city view guest room w/bb</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>886.67</v>
+      </c>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="n">
+        <v>252</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>32, 33, 34, 35, 36, 37, 28, 29, 30, 31</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>dbl/sgl mansion view guest room w/bb</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>940</v>
+      </c>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="n">
+        <v>253</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>32, 33, 34, 35, 36, 37, 28, 29, 30, 31</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>dbl/sgl e-lounge guest room w/bb</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>966.67</v>
+      </c>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="n">
+        <v>254</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>32, 33, 34, 35, 36, 37, 28, 29, 30, 31</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>dbl/sgl mansion view junior suite w/bb</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>1106.67</v>
+      </c>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="n">
+        <v>255</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>32, 33, 34, 35, 36, 37, 28, 29, 30, 31</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>dbl/sgl e-lounge junior suite w/bb</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>1153.33</v>
+      </c>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="n">
+        <v>256</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>32, 33, 34, 35, 36, 37, 28, 29, 30, 31</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>dbl/sgl city view one bedroom suite w/bb</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>1273.33</v>
+      </c>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="n">
+        <v>257</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>32, 33, 34, 35, 36, 37, 28, 29, 30, 31</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>dbl/sgl mansion view one bedroom suite w/bb</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>1326.67</v>
+      </c>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="n">
+        <v>258</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>32, 33, 34, 35, 36, 37, 28, 29, 30, 31</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026)</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Four Seasons Buenos Aires (A)</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>(Sin tipo específico)</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>dbl/sgl e-lounge one bedroom suite w/bb</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>1453.33</v>
+      </c>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="n">
+        <v>259</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>32, 33, 34, 35, 36, 37, 28, 29, 30, 31</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026) |  (01-10-2026 - 26-11-2026) |  (08-12-2026 - 23-12-2026)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="35" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Nombre</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Fecha Inicio</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Fecha Fin</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>23</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>SIN NOMBRE DE GRUPO</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>01-10-2025</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>31-10-2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>24</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SIN NOMBRE DE GRUPO</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>01-11-2025</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>26-11-2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>25</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SIN NOMBRE DE GRUPO</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>08-12-2025</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>21-12-2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>26</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SIN NOMBRE DE GRUPO</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>04-01-2026</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>31-03-2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>27</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SIN NOMBRE DE GRUPO</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>01-04-2026</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>30-09-2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>28</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SIN NOMBRE DE GRUPO</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>01-10-2026</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>26-11-2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>29</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SIN NOMBRE DE GRUPO</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>08-12-2026</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>23-12-2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>30</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SIN NOMBRE DE GRUPO</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>01-10-2026</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>26-11-2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>31</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SIN NOMBRE DE GRUPO</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>08-12-2026</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>23-12-2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>32</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>SIN NOMBRE DE GRUPO</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>01-10-2026</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>26-11-2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>33</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>SIN NOMBRE DE GRUPO</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>08-12-2026</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>23-12-2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>34</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SIN NOMBRE DE GRUPO</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>01-10-2026</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>26-11-2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>35</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>SIN NOMBRE DE GRUPO</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>08-12-2026</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>23-12-2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>36</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SIN NOMBRE DE GRUPO</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>01-10-2026</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>26-11-2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>37</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>SIN NOMBRE DE GRUPO</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>08-12-2026</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>23-12-2026</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>